<commit_message>
engage2020 username testcases has been added into excel
</commit_message>
<xml_diff>
--- a/MavenProject1/data/Testcases_for_schw15r2dw003.xlsx
+++ b/MavenProject1/data/Testcases_for_schw15r2dw003.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\MavenProject1\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17160" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Url</t>
   </si>
@@ -66,12 +62,21 @@
   </si>
   <si>
     <t>\\sselvarasuw8\screenshot\chartsNew.png</t>
+  </si>
+  <si>
+    <t>engage2020</t>
+  </si>
+  <si>
+    <t>Attrib N Risk Report</t>
+  </si>
+  <si>
+    <t>\\sselvarasuw8\screenshot\chartsNew_engage.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,16 +414,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -472,9 +477,33 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
OLAP regular one URL has changed it
</commit_message>
<xml_diff>
--- a/MavenProject1/data/Testcases_for_schw15r2dw003.xlsx
+++ b/MavenProject1/data/Testcases_for_schw15r2dw003.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17160" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15135" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>fileWithPath</t>
   </si>
   <si>
-    <t>https://schw15r2dw003.eagleinvsys.com/modules/olap/</t>
-  </si>
-  <si>
     <t>mgoodey</t>
   </si>
   <si>
@@ -71,6 +68,9 @@
   </si>
   <si>
     <t>\\sselvarasuw8\screenshot\chartsNew_engage.png</t>
+  </si>
+  <si>
+    <t>https://10.130.35.58/modules/olap/#/login</t>
   </si>
 </sst>
 </file>
@@ -414,9 +414,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -428,10 +428,13 @@
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="53.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,56 +457,57 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
     <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3" location="/login"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>